<commit_message>
Finish assignment 1 draft
</commit_message>
<xml_diff>
--- a/charles-university/data-structures-1/splay-tree/docs/results.xlsx
+++ b/charles-university/data-structures-1/splay-tree/docs/results.xlsx
@@ -26917,16 +26917,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>82562</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>177812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26956,15 +26956,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>100390</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>14665</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -27338,7 +27338,7 @@
   <dimension ref="A1:S202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>